<commit_message>
função de plotar graficos
</commit_message>
<xml_diff>
--- a/q1.xlsx
+++ b/q1.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="p1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="p2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="p3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t xml:space="preserve">x</t>
   </si>
@@ -123,8 +125,8 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="1" sqref="A3:A15 B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -236,4 +238,374 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="A3:A15 B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <f aca="false">2*A2+1</f>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">2*A3+1</f>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>-3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">2*A4+1</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>-2</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <f aca="false">2*A5+1</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <f aca="false">2*A6+1</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <f aca="false">2*A7+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <f aca="false">2*A8+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <f aca="false">2*A9+1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">2*A10+1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <f aca="false">2*A11+1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <f aca="false">2*A12+1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">2*A13+1</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">2*A14+1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">2*A15+1</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <f aca="false">2*A16+1</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <f aca="false">2*A17+1</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <f aca="false">2*A18+1</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <f aca="false">2*A19+1</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <f aca="false">2*A20+1</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <f aca="false">2*A21+1</f>
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <f aca="false">SIN(A2)</f>
+        <v>0.958924274663139</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>-4.9</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">SIN(A3)</f>
+        <v>0.982452612624332</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>-3.9</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">SIN(A4)</f>
+        <v>0.687766159183974</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>-2.9</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <f aca="false">SIN(A5)</f>
+        <v>-0.239249329213982</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <f aca="false">SIN(A6)</f>
+        <v>-0.946300087687414</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <f aca="false">SIN(A7)</f>
+        <v>-0.783326909627484</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0.0999999999999996</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <f aca="false">SIN(A8)</f>
+        <v>0.0998334166468278</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <f aca="false">SIN(A9)</f>
+        <v>0.891207360061435</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">SIN(A10)</f>
+        <v>0.863209366648874</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <f aca="false">SIN(A11)</f>
+        <v>0.0415806624332909</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <f aca="false">SIN(A12)</f>
+        <v>-0.81827711106441</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">SIN(A13)</f>
+        <v>-0.925814682327732</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">SIN(A14)</f>
+        <v>-0.182162504272096</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">SIN(A15)</f>
+        <v>0.728969040125876</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>